<commit_message>
SLR demo excel new lines
</commit_message>
<xml_diff>
--- a/_PythonNotebooks/_Course3_Machine_Learning_1/Mod1_Linear_Regression/slr_excel_demonstration_1.xlsx
+++ b/_PythonNotebooks/_Course3_Machine_Learning_1/Mod1_Linear_Regression/slr_excel_demonstration_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kumar_Data\FromD\_Upgrad\_AIML_Code\_PythonNotebooks\_Course3_Machine_Learning_1\Mod1_Linear_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E74252-93C7-4642-B6DC-FFBEE8EC879F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C8DB2-CD59-4C39-9401-5DD64A98B711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13908" yWindow="804" windowWidth="9408" windowHeight="11832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>SLOPE</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>Pred</t>
+  </si>
+  <si>
+    <t>Act-Avg</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>TSS</t>
+  </si>
+  <si>
+    <t>R2</t>
   </si>
 </sst>
 </file>
@@ -2138,15 +2150,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF14B3D2-D65F-453E-B1BE-2B618A80C9C2}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2159,8 +2171,11 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2171,8 +2186,16 @@
         <f>(A2/2)+3</f>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>(C2-B2)^2</f>
+        <v>0.25</v>
+      </c>
+      <c r="E2">
+        <f>(B2-B$8)^2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2183,8 +2206,16 @@
         <f t="shared" ref="C3:C6" si="0">(A3/2)+3</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="1">(C3-B3)^2</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="2">(B3-B$8)^2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2195,8 +2226,16 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>
@@ -2207,8 +2246,16 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -2218,6 +2265,46 @@
       <c r="C6">
         <f t="shared" si="0"/>
         <v>7</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B2:B6)</f>
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D2:D6)</f>
+        <v>6.25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <f>SUM(E2:E6)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <f>1-(D8/G8)</f>
+        <v>0.5535714285714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Linear regression session1 done
</commit_message>
<xml_diff>
--- a/_PythonNotebooks/_Course3_Machine_Learning_1/Mod1_Linear_Regression/slr_excel_demonstration_1.xlsx
+++ b/_PythonNotebooks/_Course3_Machine_Learning_1/Mod1_Linear_Regression/slr_excel_demonstration_1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kumar_Data\FromD\_Upgrad\_AIML_Code\_PythonNotebooks\_Course3_Machine_Learning_1\Mod1_Linear_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C8DB2-CD59-4C39-9401-5DD64A98B711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538D03CD-7BDD-4966-BFC3-C2D6F39A7474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13908" yWindow="804" windowWidth="9408" windowHeight="11832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>SLOPE</t>
   </si>
@@ -89,6 +90,18 @@
   </si>
   <si>
     <t>R2</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>mile</t>
+  </si>
+  <si>
+    <t>Ykm</t>
+  </si>
+  <si>
+    <t>Ymile</t>
   </si>
 </sst>
 </file>
@@ -224,16 +237,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-IN" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Actual Sales(Y) (In crores)</a:t>
+              <a:rPr lang="en-IN"/>
+              <a:t>Actual Sales(Y) (In crores) </a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-IN" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-IN" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -276,7 +282,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -336,10 +342,9 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-IN" sz="1050" b="1" baseline="0"/>
+                      <a:rPr lang="en-IN"/>
                       <a:t>y = 0.0528x + 3.3525</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-IN" sz="1050" b="1"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -790,7 +795,831 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20781933508311465"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ykm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-86DF-4943-8685-FFE85B7DDF91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="572891712"/>
+        <c:axId val="572897944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="572891712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572897944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="572897944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572891712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.89617344706911628"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ymile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>41.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>123.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>137.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2EEC-411C-A3A8-8F445BD72C9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="572871376"/>
+        <c:axId val="572876624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="572871376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572876624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="572876624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572871376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1346,6 +2175,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1357,9 +3218,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>388619</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1379,6 +3240,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2614D1FC-20B5-4BBA-86AC-5B4485E7E524}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA1EB8F6-CC9D-4136-AA63-D28446F289B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2152,7 +4090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF14B3D2-D65F-453E-B1BE-2B618A80C9C2}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2310,4 +4248,221 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C87D565-D350-404A-8592-6EDC5E467A43}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f>A2*2</f>
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <f>A2*11</f>
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <f>(B2/1.6)*11</f>
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B12" si="0">A3*2</f>
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C12" si="1">A3*11</f>
+        <v>44</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D12" si="2">(B3/1.6)*11</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>96.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>123.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>27.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>